<commit_message>
Delete something resources about the aim game.
</commit_message>
<xml_diff>
--- a/ExcelFolder/Example.xlsx
+++ b/ExcelFolder/Example.xlsx
@@ -4,17 +4,30 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12420"/>
+    <workbookView windowWidth="27945" windowHeight="12255"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="117">
   <si>
     <t>cache
 export</t>
@@ -194,7 +207,7 @@
     <t>不会被打包到代码中，只做展示</t>
   </si>
   <si>
-    <t>测试表格</t>
+    <t>测试表格1</t>
   </si>
   <si>
     <t>1,2,4</t>
@@ -219,12 +232,159 @@
   </si>
   <si>
     <t>dsadas</t>
+  </si>
+  <si>
+    <t>测试表格2</t>
+  </si>
+  <si>
+    <t>测试表格3</t>
+  </si>
+  <si>
+    <t>1,2,5</t>
+  </si>
+  <si>
+    <t>1,2.46</t>
+  </si>
+  <si>
+    <t>3,6,8</t>
+  </si>
+  <si>
+    <t>1.23,231 , 213.44,  34.34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{21, 43},{22,  3},  {232, 66 } , {231 , 223}  </t>
+  </si>
+  <si>
+    <t>测试表格4</t>
+  </si>
+  <si>
+    <t>1,2,6</t>
+  </si>
+  <si>
+    <t>1,2.47</t>
+  </si>
+  <si>
+    <t>3,6,9</t>
+  </si>
+  <si>
+    <t>1.23,231 , 213.44,  34.35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{21, 43},{22,  3},  {232, 66 } , {231 , 224}  </t>
+  </si>
+  <si>
+    <t>测试表格5</t>
+  </si>
+  <si>
+    <t>1,2,7</t>
+  </si>
+  <si>
+    <t>1,2.48</t>
+  </si>
+  <si>
+    <t>3,6,10</t>
+  </si>
+  <si>
+    <t>1.23,231 , 213.44,  34.36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{21, 43},{22,  3},  {232, 66 } , {231 , 225}  </t>
+  </si>
+  <si>
+    <t>测试表格6</t>
+  </si>
+  <si>
+    <t>1,2,8</t>
+  </si>
+  <si>
+    <t>1,2.49</t>
+  </si>
+  <si>
+    <t>3,6,11</t>
+  </si>
+  <si>
+    <t>1.23,231 , 213.44,  34.37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{21, 43},{22,  3},  {232, 66 } , {231 , 226}  </t>
+  </si>
+  <si>
+    <t>测试表格7</t>
+  </si>
+  <si>
+    <t>1,2,9</t>
+  </si>
+  <si>
+    <t>1,2.50</t>
+  </si>
+  <si>
+    <t>3,6,12</t>
+  </si>
+  <si>
+    <t>1.23,231 , 213.44,  34.38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{21, 43},{22,  3},  {232, 66 } , {231 , 227}  </t>
+  </si>
+  <si>
+    <t>测试表格8</t>
+  </si>
+  <si>
+    <t>1,2,10</t>
+  </si>
+  <si>
+    <t>1,2.51</t>
+  </si>
+  <si>
+    <t>3,6,13</t>
+  </si>
+  <si>
+    <t>1.23,231 , 213.44,  34.39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{21, 43},{22,  3},  {232, 66 } , {231 , 228}  </t>
+  </si>
+  <si>
+    <t>测试表格9</t>
+  </si>
+  <si>
+    <t>1,2,11</t>
+  </si>
+  <si>
+    <t>1,2.52</t>
+  </si>
+  <si>
+    <t>3,6,14</t>
+  </si>
+  <si>
+    <t>1.23,231 , 213.44,  34.40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{21, 43},{22,  3},  {232, 66 } , {231 , 229}  </t>
+  </si>
+  <si>
+    <t>测试表格10</t>
+  </si>
+  <si>
+    <t>1,2,12</t>
+  </si>
+  <si>
+    <t>1,2.53</t>
+  </si>
+  <si>
+    <t>3,6,15</t>
+  </si>
+  <si>
+    <t>1.23,231 , 213.44,  34.41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{21, 43},{22,  3},  {232, 66 } , {231 , 230}  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -246,34 +406,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -287,14 +419,6 @@
       <color rgb="FF800080"/>
       <name val="等线"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -334,6 +458,21 @@
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -384,7 +523,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -417,49 +577,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -471,121 +715,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,21 +768,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -655,6 +800,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -711,148 +871,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -877,52 +1037,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="百分比" xfId="3" builtinId="5"/>
+    <cellStyle name="千位分隔[0]" xfId="4" builtinId="6"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
+    <cellStyle name="超链接" xfId="6" builtinId="8"/>
+    <cellStyle name="已访问的超链接" xfId="7" builtinId="9"/>
+    <cellStyle name="注释" xfId="8" builtinId="10"/>
+    <cellStyle name="警告文本" xfId="9" builtinId="11"/>
+    <cellStyle name="标题" xfId="10" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="11" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="12" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="13" builtinId="17"/>
+    <cellStyle name="标题 3" xfId="14" builtinId="18"/>
     <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="输入" xfId="16" builtinId="20"/>
+    <cellStyle name="输出" xfId="17" builtinId="21"/>
+    <cellStyle name="计算" xfId="18" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="19" builtinId="23"/>
+    <cellStyle name="链接单元格" xfId="20" builtinId="24"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="好" xfId="22" builtinId="26"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="适中" xfId="24" builtinId="28"/>
+    <cellStyle name="强调文字颜色 1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="28" builtinId="32"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="32" builtinId="36"/>
+    <cellStyle name="强调文字颜色 3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="强调文字颜色 4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="40" builtinId="44"/>
+    <cellStyle name="强调文字颜色 5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="44" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1193,15 +1353,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:V15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="9.5" style="3" customWidth="1"/>
     <col min="2" max="2" width="7" style="4" customWidth="1"/>
@@ -1538,6 +1698,489 @@
         <v>34.22</v>
       </c>
     </row>
+    <row r="7" spans="2:22">
+      <c r="B7" s="4">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K7" s="4">
+        <v>1</v>
+      </c>
+      <c r="L7" s="4">
+        <v>2</v>
+      </c>
+      <c r="M7" s="4">
+        <v>3</v>
+      </c>
+      <c r="N7" s="4">
+        <v>4</v>
+      </c>
+      <c r="O7" s="4">
+        <v>5</v>
+      </c>
+      <c r="P7" s="4">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>7</v>
+      </c>
+      <c r="T7" s="4">
+        <v>3.444</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="V7" s="4">
+        <v>34.22</v>
+      </c>
+    </row>
+    <row r="8" spans="2:20">
+      <c r="B8" s="4">
+        <v>3</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K8" s="4">
+        <v>2</v>
+      </c>
+      <c r="L8" s="4">
+        <v>3</v>
+      </c>
+      <c r="M8" s="4">
+        <v>4</v>
+      </c>
+      <c r="N8" s="4">
+        <v>5</v>
+      </c>
+      <c r="O8" s="4">
+        <v>6</v>
+      </c>
+      <c r="P8" s="4">
+        <v>7</v>
+      </c>
+      <c r="Q8" s="4">
+        <v>8</v>
+      </c>
+      <c r="T8" s="4">
+        <v>4.444</v>
+      </c>
+    </row>
+    <row r="9" spans="2:20">
+      <c r="B9" s="4">
+        <v>4</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K9" s="4">
+        <v>3</v>
+      </c>
+      <c r="L9" s="4">
+        <v>4</v>
+      </c>
+      <c r="M9" s="4">
+        <v>5</v>
+      </c>
+      <c r="N9" s="4">
+        <v>6</v>
+      </c>
+      <c r="O9" s="4">
+        <v>7</v>
+      </c>
+      <c r="P9" s="4">
+        <v>8</v>
+      </c>
+      <c r="Q9" s="4">
+        <v>9</v>
+      </c>
+      <c r="T9" s="4">
+        <v>5.444</v>
+      </c>
+    </row>
+    <row r="10" spans="2:20">
+      <c r="B10" s="4">
+        <v>5</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K10" s="4">
+        <v>4</v>
+      </c>
+      <c r="L10" s="4">
+        <v>5</v>
+      </c>
+      <c r="M10" s="4">
+        <v>6</v>
+      </c>
+      <c r="N10" s="4">
+        <v>7</v>
+      </c>
+      <c r="O10" s="4">
+        <v>8</v>
+      </c>
+      <c r="P10" s="4">
+        <v>9</v>
+      </c>
+      <c r="Q10" s="4">
+        <v>10</v>
+      </c>
+      <c r="T10" s="4">
+        <v>6.444</v>
+      </c>
+    </row>
+    <row r="11" spans="2:20">
+      <c r="B11" s="4">
+        <v>6</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K11" s="4">
+        <v>5</v>
+      </c>
+      <c r="L11" s="4">
+        <v>6</v>
+      </c>
+      <c r="M11" s="4">
+        <v>7</v>
+      </c>
+      <c r="N11" s="4">
+        <v>8</v>
+      </c>
+      <c r="O11" s="4">
+        <v>9</v>
+      </c>
+      <c r="P11" s="4">
+        <v>10</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>11</v>
+      </c>
+      <c r="T11" s="4">
+        <v>7.444</v>
+      </c>
+    </row>
+    <row r="12" spans="2:20">
+      <c r="B12" s="4">
+        <v>7</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K12" s="4">
+        <v>6</v>
+      </c>
+      <c r="L12" s="4">
+        <v>7</v>
+      </c>
+      <c r="M12" s="4">
+        <v>8</v>
+      </c>
+      <c r="N12" s="4">
+        <v>9</v>
+      </c>
+      <c r="O12" s="4">
+        <v>10</v>
+      </c>
+      <c r="P12" s="4">
+        <v>11</v>
+      </c>
+      <c r="Q12" s="4">
+        <v>12</v>
+      </c>
+      <c r="T12" s="4">
+        <v>8.444</v>
+      </c>
+    </row>
+    <row r="13" spans="2:20">
+      <c r="B13" s="4">
+        <v>8</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K13" s="4">
+        <v>7</v>
+      </c>
+      <c r="L13" s="4">
+        <v>8</v>
+      </c>
+      <c r="M13" s="4">
+        <v>9</v>
+      </c>
+      <c r="N13" s="4">
+        <v>10</v>
+      </c>
+      <c r="O13" s="4">
+        <v>11</v>
+      </c>
+      <c r="P13" s="4">
+        <v>12</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>13</v>
+      </c>
+      <c r="T13" s="4">
+        <v>9.444</v>
+      </c>
+    </row>
+    <row r="14" spans="2:20">
+      <c r="B14" s="4">
+        <v>9</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K14" s="4">
+        <v>8</v>
+      </c>
+      <c r="L14" s="4">
+        <v>9</v>
+      </c>
+      <c r="M14" s="4">
+        <v>10</v>
+      </c>
+      <c r="N14" s="4">
+        <v>11</v>
+      </c>
+      <c r="O14" s="4">
+        <v>12</v>
+      </c>
+      <c r="P14" s="4">
+        <v>13</v>
+      </c>
+      <c r="Q14" s="4">
+        <v>14</v>
+      </c>
+      <c r="T14" s="4">
+        <v>10.444</v>
+      </c>
+    </row>
+    <row r="15" spans="2:20">
+      <c r="B15" s="4">
+        <v>10</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="K15" s="4">
+        <v>9</v>
+      </c>
+      <c r="L15" s="4">
+        <v>10</v>
+      </c>
+      <c r="M15" s="4">
+        <v>11</v>
+      </c>
+      <c r="N15" s="4">
+        <v>12</v>
+      </c>
+      <c r="O15" s="4">
+        <v>13</v>
+      </c>
+      <c r="P15" s="4">
+        <v>14</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>15</v>
+      </c>
+      <c r="T15" s="4">
+        <v>11.444</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>